<commit_message>
Doing latest commit before I pull from Iddo's branch.
</commit_message>
<xml_diff>
--- a/Final Data/FinalData.xlsx
+++ b/Final Data/FinalData.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20100" tabRatio="500" activeTab="2"/>
-    <workbookView xWindow="8240" yWindow="0" windowWidth="25220" windowHeight="19780" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19420" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="List top 50 Papers" sheetId="1" r:id="rId1"/>
     <sheet name="Prots&amp;AnnotsTaxid" sheetId="2" r:id="rId2"/>
     <sheet name="allExpTaxonIDsTop50.txt" sheetId="3" r:id="rId3"/>
+    <sheet name="Sort Top 50 for species" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="432">
   <si>
     <t>Num Prots</t>
   </si>
@@ -1312,6 +1312,12 @@
   </si>
   <si>
     <t>Pombe</t>
+  </si>
+  <si>
+    <t>Annotation Coverage</t>
+  </si>
+  <si>
+    <t>Paper Count</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1628,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1666,8 +1672,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1711,8 +1729,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1753,11 +1772,23 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1765,47 +1796,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1842,6 +1832,37 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -1853,6 +1874,348 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sort Top 50 for species'!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Annotation Coverage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sort Top 50 for species'!$R$2:$R$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Arabidopsis thaliana</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Caenorhabditis elegans</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dictyostelium discoideum</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Drosophila melanogaster</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Human</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mouse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mycobacterium tuberculosis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pombe</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Saccharomyces cerevisiae S288c</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sort Top 50 for species'!$T$2:$T$10</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.233151803948264</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.524788930581613</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0743674367436744</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.034448904790994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.165292322915808</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0249011369253584</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.391599307159353</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.464310684548401</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.121951219512195</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="958707816"/>
+        <c:axId val="958709608"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sort Top 50 for species'!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Paper Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sort Top 50 for species'!$R$2:$R$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Arabidopsis thaliana</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Caenorhabditis elegans</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dictyostelium discoideum</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Drosophila melanogaster</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Human</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Mouse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Mycobacterium tuberculosis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Pombe</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Saccharomyces cerevisiae S288c</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sort Top 50 for species'!$S$2:$S$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="958713496"/>
+        <c:axId val="958711416"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="958707816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="958709608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="958709608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="958707816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="958711416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="958713496"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="958713496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="958711416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2179,10 +2542,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EB52"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
-    <sheetView showRuler="0" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -8501,39 +8863,39 @@
         <v>64542</v>
       </c>
       <c r="H52" s="34">
-        <f>SUM(H2:H51)</f>
+        <f t="shared" ref="H52:P52" si="0">SUM(H2:H51)</f>
         <v>1581</v>
       </c>
       <c r="I52" s="35">
-        <f>SUM(I2:I51)</f>
+        <f t="shared" si="0"/>
         <v>24241</v>
       </c>
       <c r="J52" s="36">
-        <f>SUM(J2:J51)</f>
+        <f t="shared" si="0"/>
         <v>38720</v>
       </c>
       <c r="K52" s="37">
-        <f>SUM(K2:K51)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L52" s="38">
-        <f>SUM(L2:L51)</f>
+        <f t="shared" si="0"/>
         <v>38721</v>
       </c>
       <c r="M52" s="38">
-        <f>SUM(M2:M51)</f>
+        <f t="shared" si="0"/>
         <v>519</v>
       </c>
       <c r="N52" s="38">
-        <f>SUM(N2:N51)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O52" s="38">
-        <f>SUM(O2:O51)</f>
+        <f t="shared" si="0"/>
         <v>23722</v>
       </c>
       <c r="P52" s="39">
-        <f>SUM(P2:P51)</f>
+        <f t="shared" si="0"/>
         <v>1580</v>
       </c>
     </row>
@@ -8542,7 +8904,6 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -8553,10 +8914,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D957"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A909" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
-    <sheetView showRuler="0" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -19143,7 +19503,6 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -19154,11 +19513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
-    </sheetView>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="1">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F27" sqref="A1:O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21409,7 +21765,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThanOrEqual">
       <formula>20</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThanOrEqual">
@@ -21420,7 +21776,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThanOrEqual">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21429,6 +21785,2397 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="8" max="8" width="30" customWidth="1"/>
+    <col min="18" max="18" width="22.1640625" customWidth="1"/>
+    <col min="20" max="20" width="14.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>424</v>
+      </c>
+      <c r="H1" t="s">
+        <v>412</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>425</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>426</v>
+      </c>
+      <c r="N1" t="s">
+        <v>427</v>
+      </c>
+      <c r="O1" s="41" t="s">
+        <v>428</v>
+      </c>
+      <c r="R1" t="s">
+        <v>412</v>
+      </c>
+      <c r="S1" t="s">
+        <v>431</v>
+      </c>
+      <c r="T1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2">
+        <v>1251</v>
+      </c>
+      <c r="B2">
+        <v>1251</v>
+      </c>
+      <c r="C2">
+        <v>18431481</v>
+      </c>
+      <c r="D2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2">
+        <v>2008</v>
+      </c>
+      <c r="F2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H2" t="s">
+        <v>407</v>
+      </c>
+      <c r="I2">
+        <v>1251</v>
+      </c>
+      <c r="L2">
+        <v>10153</v>
+      </c>
+      <c r="M2" s="41">
+        <f t="shared" ref="M2:M33" si="0">A2/L2*100</f>
+        <v>12.321481335565842</v>
+      </c>
+      <c r="N2">
+        <v>41132</v>
+      </c>
+      <c r="O2" s="41">
+        <f t="shared" ref="O2:O33" si="1">B2/N2*100</f>
+        <v>3.0414275989497228</v>
+      </c>
+      <c r="R2" t="s">
+        <v>407</v>
+      </c>
+      <c r="S2">
+        <f>COUNTA(H2:H17)</f>
+        <v>16</v>
+      </c>
+      <c r="T2" s="43">
+        <f>SUM(B2:B17)/41132</f>
+        <v>0.23315180394826412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3">
+        <v>1136</v>
+      </c>
+      <c r="B3">
+        <v>1136</v>
+      </c>
+      <c r="C3">
+        <v>17317660</v>
+      </c>
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3">
+        <v>2007</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>362</v>
+      </c>
+      <c r="H3" t="s">
+        <v>407</v>
+      </c>
+      <c r="I3">
+        <v>1136</v>
+      </c>
+      <c r="L3">
+        <v>10153</v>
+      </c>
+      <c r="M3" s="41">
+        <f t="shared" si="0"/>
+        <v>11.188811188811188</v>
+      </c>
+      <c r="N3">
+        <v>41132</v>
+      </c>
+      <c r="O3" s="41">
+        <f t="shared" si="1"/>
+        <v>2.7618399299815231</v>
+      </c>
+      <c r="R3" t="s">
+        <v>409</v>
+      </c>
+      <c r="S3">
+        <f>COUNTA(H18:H29)</f>
+        <v>12</v>
+      </c>
+      <c r="T3" s="43">
+        <f>SUM(B18:B29)/42640</f>
+        <v>0.52478893058161347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4">
+        <v>1041</v>
+      </c>
+      <c r="B4">
+        <v>1041</v>
+      </c>
+      <c r="C4">
+        <v>21166475</v>
+      </c>
+      <c r="D4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E4">
+        <v>2011</v>
+      </c>
+      <c r="F4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" t="s">
+        <v>362</v>
+      </c>
+      <c r="H4" t="s">
+        <v>407</v>
+      </c>
+      <c r="I4">
+        <v>1041</v>
+      </c>
+      <c r="L4">
+        <v>10153</v>
+      </c>
+      <c r="M4" s="41">
+        <f t="shared" si="0"/>
+        <v>10.253127154535607</v>
+      </c>
+      <c r="N4">
+        <v>41132</v>
+      </c>
+      <c r="O4" s="41">
+        <f t="shared" si="1"/>
+        <v>2.5308762034425754</v>
+      </c>
+      <c r="R4" t="s">
+        <v>417</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4" s="43">
+        <f>B30/'Prots&amp;AnnotsTaxid'!B14</f>
+        <v>7.4367436743674367E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5">
+        <v>784</v>
+      </c>
+      <c r="B5">
+        <v>784</v>
+      </c>
+      <c r="C5">
+        <v>21533090</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5">
+        <v>2011</v>
+      </c>
+      <c r="F5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" t="s">
+        <v>362</v>
+      </c>
+      <c r="H5" t="s">
+        <v>407</v>
+      </c>
+      <c r="I5">
+        <v>784</v>
+      </c>
+      <c r="L5">
+        <v>10153</v>
+      </c>
+      <c r="M5" s="41">
+        <f t="shared" si="0"/>
+        <v>7.7218556091795527</v>
+      </c>
+      <c r="N5">
+        <v>41132</v>
+      </c>
+      <c r="O5" s="41">
+        <f t="shared" si="1"/>
+        <v>1.9060585432266848</v>
+      </c>
+      <c r="R5" t="s">
+        <v>408</v>
+      </c>
+      <c r="S5">
+        <f>COUNTA(H31:H34)</f>
+        <v>4</v>
+      </c>
+      <c r="T5" s="43">
+        <f>SUM(B31:B34)/'Prots&amp;AnnotsTaxid'!B6</f>
+        <v>3.4448904790993981E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6">
+        <v>724</v>
+      </c>
+      <c r="B6">
+        <v>882</v>
+      </c>
+      <c r="C6">
+        <v>20061580</v>
+      </c>
+      <c r="D6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6">
+        <v>2010</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>362</v>
+      </c>
+      <c r="H6" t="s">
+        <v>407</v>
+      </c>
+      <c r="I6">
+        <v>882</v>
+      </c>
+      <c r="L6">
+        <v>10153</v>
+      </c>
+      <c r="M6" s="41">
+        <f t="shared" si="0"/>
+        <v>7.1308972717423424</v>
+      </c>
+      <c r="N6">
+        <v>41132</v>
+      </c>
+      <c r="O6" s="41">
+        <f t="shared" si="1"/>
+        <v>2.1443158611300204</v>
+      </c>
+      <c r="R6" t="s">
+        <v>406</v>
+      </c>
+      <c r="S6">
+        <f>COUNTA(H35:H37)</f>
+        <v>3</v>
+      </c>
+      <c r="T6" s="43">
+        <f>SUM(B35:B37)/'Prots&amp;AnnotsTaxid'!B4</f>
+        <v>0.1652923229158077</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7">
+        <v>634</v>
+      </c>
+      <c r="B7">
+        <v>634</v>
+      </c>
+      <c r="C7">
+        <v>15028209</v>
+      </c>
+      <c r="D7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7">
+        <v>2004</v>
+      </c>
+      <c r="F7" t="s">
+        <v>188</v>
+      </c>
+      <c r="G7" t="s">
+        <v>362</v>
+      </c>
+      <c r="H7" t="s">
+        <v>407</v>
+      </c>
+      <c r="I7">
+        <v>634</v>
+      </c>
+      <c r="L7">
+        <v>10153</v>
+      </c>
+      <c r="M7" s="41">
+        <f t="shared" si="0"/>
+        <v>6.2444597655865266</v>
+      </c>
+      <c r="N7">
+        <v>41132</v>
+      </c>
+      <c r="O7" s="41">
+        <f t="shared" si="1"/>
+        <v>1.5413789750072937</v>
+      </c>
+      <c r="R7" t="s">
+        <v>405</v>
+      </c>
+      <c r="S7">
+        <f>COUNTA(H38:H41)</f>
+        <v>4</v>
+      </c>
+      <c r="T7" s="43">
+        <f>SUM(I38:I41)/'Prots&amp;AnnotsTaxid'!B3</f>
+        <v>2.4901136925358378E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8">
+        <v>577</v>
+      </c>
+      <c r="B8">
+        <v>577</v>
+      </c>
+      <c r="C8">
+        <v>17432890</v>
+      </c>
+      <c r="D8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8">
+        <v>2007</v>
+      </c>
+      <c r="F8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G8" t="s">
+        <v>362</v>
+      </c>
+      <c r="H8" t="s">
+        <v>407</v>
+      </c>
+      <c r="I8">
+        <v>577</v>
+      </c>
+      <c r="L8">
+        <v>10153</v>
+      </c>
+      <c r="M8" s="41">
+        <f t="shared" si="0"/>
+        <v>5.6830493450211756</v>
+      </c>
+      <c r="N8">
+        <v>41132</v>
+      </c>
+      <c r="O8" s="41">
+        <f t="shared" si="1"/>
+        <v>1.4028007390839248</v>
+      </c>
+      <c r="R8" t="s">
+        <v>415</v>
+      </c>
+      <c r="S8">
+        <f>COUNTA(H42:H44)</f>
+        <v>3</v>
+      </c>
+      <c r="T8" s="43">
+        <f>SUM(B42:B44)/'Prots&amp;AnnotsTaxid'!B12</f>
+        <v>0.39159930715935337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9">
+        <v>436</v>
+      </c>
+      <c r="B9">
+        <v>436</v>
+      </c>
+      <c r="C9">
+        <v>17644812</v>
+      </c>
+      <c r="D9" t="s">
+        <v>236</v>
+      </c>
+      <c r="E9">
+        <v>2007</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>362</v>
+      </c>
+      <c r="H9" t="s">
+        <v>407</v>
+      </c>
+      <c r="I9">
+        <v>436</v>
+      </c>
+      <c r="L9">
+        <v>10153</v>
+      </c>
+      <c r="M9" s="41">
+        <f t="shared" si="0"/>
+        <v>4.294297252043731</v>
+      </c>
+      <c r="N9">
+        <v>41132</v>
+      </c>
+      <c r="O9" s="41">
+        <f t="shared" si="1"/>
+        <v>1.0600019449576972</v>
+      </c>
+      <c r="R9" t="s">
+        <v>429</v>
+      </c>
+      <c r="S9">
+        <f>COUNTA(H45:H46)</f>
+        <v>2</v>
+      </c>
+      <c r="T9" s="43">
+        <f>SUM(B45:B46)/'Prots&amp;AnnotsTaxid'!B11</f>
+        <v>0.46431068454840146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10">
+        <v>430</v>
+      </c>
+      <c r="B10">
+        <v>513</v>
+      </c>
+      <c r="C10">
+        <v>16618929</v>
+      </c>
+      <c r="D10" t="s">
+        <v>237</v>
+      </c>
+      <c r="E10">
+        <v>2006</v>
+      </c>
+      <c r="F10" t="s">
+        <v>208</v>
+      </c>
+      <c r="G10" t="s">
+        <v>362</v>
+      </c>
+      <c r="H10" t="s">
+        <v>407</v>
+      </c>
+      <c r="I10">
+        <v>513</v>
+      </c>
+      <c r="L10">
+        <v>10153</v>
+      </c>
+      <c r="M10" s="41">
+        <f t="shared" si="0"/>
+        <v>4.2352014183000097</v>
+      </c>
+      <c r="N10">
+        <v>41132</v>
+      </c>
+      <c r="O10" s="41">
+        <f t="shared" si="1"/>
+        <v>1.2472041233103182</v>
+      </c>
+      <c r="R10" t="s">
+        <v>410</v>
+      </c>
+      <c r="S10">
+        <f>COUNTA(H47:H51)</f>
+        <v>5</v>
+      </c>
+      <c r="T10" s="43">
+        <f>SUM(B47:B51)/'Prots&amp;AnnotsTaxid'!B8</f>
+        <v>0.12195121951219512</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11">
+        <v>401</v>
+      </c>
+      <c r="B11">
+        <v>401</v>
+      </c>
+      <c r="C11">
+        <v>17151019</v>
+      </c>
+      <c r="D11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E11">
+        <v>2007</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>362</v>
+      </c>
+      <c r="H11" t="s">
+        <v>407</v>
+      </c>
+      <c r="I11">
+        <v>401</v>
+      </c>
+      <c r="L11">
+        <v>10153</v>
+      </c>
+      <c r="M11" s="41">
+        <f t="shared" si="0"/>
+        <v>3.9495715552053579</v>
+      </c>
+      <c r="N11">
+        <v>41132</v>
+      </c>
+      <c r="O11" s="41">
+        <f t="shared" si="1"/>
+        <v>0.97491004570650597</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12">
+        <v>392</v>
+      </c>
+      <c r="B12">
+        <v>392</v>
+      </c>
+      <c r="C12">
+        <v>14671022</v>
+      </c>
+      <c r="D12" t="s">
+        <v>254</v>
+      </c>
+      <c r="E12">
+        <v>2004</v>
+      </c>
+      <c r="F12" t="s">
+        <v>255</v>
+      </c>
+      <c r="G12" t="s">
+        <v>362</v>
+      </c>
+      <c r="H12" t="s">
+        <v>407</v>
+      </c>
+      <c r="I12">
+        <v>392</v>
+      </c>
+      <c r="L12">
+        <v>10153</v>
+      </c>
+      <c r="M12" s="41">
+        <f t="shared" si="0"/>
+        <v>3.8609278045897764</v>
+      </c>
+      <c r="N12">
+        <v>41132</v>
+      </c>
+      <c r="O12" s="41">
+        <f t="shared" si="1"/>
+        <v>0.95302927161334239</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13">
+        <v>380</v>
+      </c>
+      <c r="B13">
+        <v>380</v>
+      </c>
+      <c r="C13">
+        <v>15539469</v>
+      </c>
+      <c r="D13" t="s">
+        <v>266</v>
+      </c>
+      <c r="E13">
+        <v>2004</v>
+      </c>
+      <c r="F13" t="s">
+        <v>255</v>
+      </c>
+      <c r="G13" t="s">
+        <v>362</v>
+      </c>
+      <c r="H13" t="s">
+        <v>407</v>
+      </c>
+      <c r="I13">
+        <v>380</v>
+      </c>
+      <c r="L13">
+        <v>10153</v>
+      </c>
+      <c r="M13" s="41">
+        <f t="shared" si="0"/>
+        <v>3.7427361371023342</v>
+      </c>
+      <c r="N13">
+        <v>41132</v>
+      </c>
+      <c r="O13" s="41">
+        <f t="shared" si="1"/>
+        <v>0.92385490615579124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14">
+        <v>328</v>
+      </c>
+      <c r="B14">
+        <v>328</v>
+      </c>
+      <c r="C14">
+        <v>12938931</v>
+      </c>
+      <c r="D14" t="s">
+        <v>280</v>
+      </c>
+      <c r="E14">
+        <v>2003</v>
+      </c>
+      <c r="F14" t="s">
+        <v>168</v>
+      </c>
+      <c r="G14" t="s">
+        <v>362</v>
+      </c>
+      <c r="H14" t="s">
+        <v>407</v>
+      </c>
+      <c r="I14">
+        <v>328</v>
+      </c>
+      <c r="L14">
+        <v>10153</v>
+      </c>
+      <c r="M14" s="41">
+        <f t="shared" si="0"/>
+        <v>3.2305722446567513</v>
+      </c>
+      <c r="N14">
+        <v>41132</v>
+      </c>
+      <c r="O14" s="41">
+        <f t="shared" si="1"/>
+        <v>0.79743265583973544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15">
+        <v>305</v>
+      </c>
+      <c r="B15">
+        <v>312</v>
+      </c>
+      <c r="C15">
+        <v>18633119</v>
+      </c>
+      <c r="D15" t="s">
+        <v>292</v>
+      </c>
+      <c r="E15">
+        <v>2008</v>
+      </c>
+      <c r="F15" t="s">
+        <v>293</v>
+      </c>
+      <c r="G15" t="s">
+        <v>362</v>
+      </c>
+      <c r="H15" t="s">
+        <v>407</v>
+      </c>
+      <c r="I15">
+        <v>312</v>
+      </c>
+      <c r="L15">
+        <v>10153</v>
+      </c>
+      <c r="M15" s="41">
+        <f t="shared" si="0"/>
+        <v>3.0040382153058207</v>
+      </c>
+      <c r="N15">
+        <v>41132</v>
+      </c>
+      <c r="O15" s="41">
+        <f t="shared" si="1"/>
+        <v>0.75853350189633373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16">
+        <v>260</v>
+      </c>
+      <c r="B16">
+        <v>260</v>
+      </c>
+      <c r="C16">
+        <v>16502469</v>
+      </c>
+      <c r="D16" t="s">
+        <v>309</v>
+      </c>
+      <c r="E16">
+        <v>2006</v>
+      </c>
+      <c r="F16" t="s">
+        <v>277</v>
+      </c>
+      <c r="G16" t="s">
+        <v>362</v>
+      </c>
+      <c r="H16" t="s">
+        <v>407</v>
+      </c>
+      <c r="I16">
+        <v>260</v>
+      </c>
+      <c r="L16">
+        <v>10153</v>
+      </c>
+      <c r="M16" s="41">
+        <f t="shared" si="0"/>
+        <v>2.5608194622279128</v>
+      </c>
+      <c r="N16">
+        <v>41132</v>
+      </c>
+      <c r="O16" s="41">
+        <f t="shared" si="1"/>
+        <v>0.63211125158027814</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17">
+        <v>241</v>
+      </c>
+      <c r="B17">
+        <v>263</v>
+      </c>
+      <c r="C17">
+        <v>16287169</v>
+      </c>
+      <c r="D17" t="s">
+        <v>354</v>
+      </c>
+      <c r="E17">
+        <v>2006</v>
+      </c>
+      <c r="F17" t="s">
+        <v>277</v>
+      </c>
+      <c r="G17" t="s">
+        <v>362</v>
+      </c>
+      <c r="H17" t="s">
+        <v>407</v>
+      </c>
+      <c r="I17">
+        <v>263</v>
+      </c>
+      <c r="L17">
+        <v>10153</v>
+      </c>
+      <c r="M17" s="41">
+        <f t="shared" si="0"/>
+        <v>2.3736826553727961</v>
+      </c>
+      <c r="N17">
+        <v>41132</v>
+      </c>
+      <c r="O17" s="41">
+        <f t="shared" si="1"/>
+        <v>0.63940484294466604</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18">
+        <v>1791</v>
+      </c>
+      <c r="B18">
+        <v>5918</v>
+      </c>
+      <c r="C18">
+        <v>14551910</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18">
+        <v>2003</v>
+      </c>
+      <c r="F18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" t="s">
+        <v>364</v>
+      </c>
+      <c r="H18" t="s">
+        <v>409</v>
+      </c>
+      <c r="I18">
+        <v>5915</v>
+      </c>
+      <c r="J18" t="s">
+        <v>370</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <v>5302</v>
+      </c>
+      <c r="M18" s="41">
+        <f t="shared" si="0"/>
+        <v>33.779705771407016</v>
+      </c>
+      <c r="N18">
+        <v>42640</v>
+      </c>
+      <c r="O18" s="41">
+        <f t="shared" si="1"/>
+        <v>13.878986866791745</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19">
+        <v>1205</v>
+      </c>
+      <c r="B19">
+        <v>1476</v>
+      </c>
+      <c r="C19">
+        <v>15791247</v>
+      </c>
+      <c r="D19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19">
+        <v>2005</v>
+      </c>
+      <c r="F19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" t="s">
+        <v>364</v>
+      </c>
+      <c r="H19" t="s">
+        <v>409</v>
+      </c>
+      <c r="I19">
+        <v>1476</v>
+      </c>
+      <c r="L19">
+        <v>5302</v>
+      </c>
+      <c r="M19" s="41">
+        <f t="shared" si="0"/>
+        <v>22.727272727272727</v>
+      </c>
+      <c r="N19">
+        <v>42640</v>
+      </c>
+      <c r="O19" s="41">
+        <f t="shared" si="1"/>
+        <v>3.4615384615384617</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20">
+        <v>1101</v>
+      </c>
+      <c r="B20">
+        <v>2269</v>
+      </c>
+      <c r="C20">
+        <v>12529635</v>
+      </c>
+      <c r="D20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20">
+        <v>2003</v>
+      </c>
+      <c r="F20" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" t="s">
+        <v>364</v>
+      </c>
+      <c r="H20" t="s">
+        <v>409</v>
+      </c>
+      <c r="I20">
+        <v>2265</v>
+      </c>
+      <c r="J20" t="s">
+        <v>370</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>5302</v>
+      </c>
+      <c r="M20" s="41">
+        <f t="shared" si="0"/>
+        <v>20.76574877404753</v>
+      </c>
+      <c r="N20">
+        <v>42640</v>
+      </c>
+      <c r="O20" s="41">
+        <f t="shared" si="1"/>
+        <v>5.3212945590994369</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21">
+        <v>865</v>
+      </c>
+      <c r="B21">
+        <v>1533</v>
+      </c>
+      <c r="C21">
+        <v>15489339</v>
+      </c>
+      <c r="D21" t="s">
+        <v>169</v>
+      </c>
+      <c r="E21">
+        <v>2004</v>
+      </c>
+      <c r="F21" t="s">
+        <v>170</v>
+      </c>
+      <c r="G21" t="s">
+        <v>364</v>
+      </c>
+      <c r="H21" t="s">
+        <v>409</v>
+      </c>
+      <c r="I21">
+        <v>1532</v>
+      </c>
+      <c r="J21" t="s">
+        <v>370</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>5302</v>
+      </c>
+      <c r="M21" s="41">
+        <f t="shared" si="0"/>
+        <v>16.314598264805731</v>
+      </c>
+      <c r="N21">
+        <v>42640</v>
+      </c>
+      <c r="O21" s="41">
+        <f t="shared" si="1"/>
+        <v>3.5952157598499062</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22">
+        <v>607</v>
+      </c>
+      <c r="B22">
+        <v>661</v>
+      </c>
+      <c r="C22">
+        <v>17704769</v>
+      </c>
+      <c r="D22" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22">
+        <v>2007</v>
+      </c>
+      <c r="F22" t="s">
+        <v>192</v>
+      </c>
+      <c r="G22" t="s">
+        <v>364</v>
+      </c>
+      <c r="H22" t="s">
+        <v>409</v>
+      </c>
+      <c r="I22">
+        <v>660</v>
+      </c>
+      <c r="J22" t="s">
+        <v>370</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>5302</v>
+      </c>
+      <c r="M22" s="41">
+        <f t="shared" si="0"/>
+        <v>11.448509996227839</v>
+      </c>
+      <c r="N22">
+        <v>42640</v>
+      </c>
+      <c r="O22" s="41">
+        <f t="shared" si="1"/>
+        <v>1.550187617260788</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23">
+        <v>553</v>
+      </c>
+      <c r="B23">
+        <v>884</v>
+      </c>
+      <c r="C23">
+        <v>11231151</v>
+      </c>
+      <c r="D23" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23">
+        <v>2001</v>
+      </c>
+      <c r="F23" t="s">
+        <v>188</v>
+      </c>
+      <c r="G23" t="s">
+        <v>364</v>
+      </c>
+      <c r="H23" t="s">
+        <v>409</v>
+      </c>
+      <c r="I23">
+        <v>884</v>
+      </c>
+      <c r="L23">
+        <v>5302</v>
+      </c>
+      <c r="M23" s="41">
+        <f t="shared" si="0"/>
+        <v>10.430026405130139</v>
+      </c>
+      <c r="N23">
+        <v>42640</v>
+      </c>
+      <c r="O23" s="41">
+        <f t="shared" si="1"/>
+        <v>2.0731707317073171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24">
+        <v>516</v>
+      </c>
+      <c r="B24">
+        <v>5972</v>
+      </c>
+      <c r="C24">
+        <v>17417969</v>
+      </c>
+      <c r="D24" t="s">
+        <v>205</v>
+      </c>
+      <c r="E24">
+        <v>2007</v>
+      </c>
+      <c r="F24" t="s">
+        <v>206</v>
+      </c>
+      <c r="G24" t="s">
+        <v>364</v>
+      </c>
+      <c r="H24" t="s">
+        <v>409</v>
+      </c>
+      <c r="I24">
+        <v>5972</v>
+      </c>
+      <c r="L24">
+        <v>5302</v>
+      </c>
+      <c r="M24" s="41">
+        <f t="shared" si="0"/>
+        <v>9.7321765371557909</v>
+      </c>
+      <c r="N24">
+        <v>42640</v>
+      </c>
+      <c r="O24" s="41">
+        <f t="shared" si="1"/>
+        <v>14.00562851782364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25">
+        <v>479</v>
+      </c>
+      <c r="B25">
+        <v>848</v>
+      </c>
+      <c r="C25">
+        <v>21529718</v>
+      </c>
+      <c r="D25" t="s">
+        <v>213</v>
+      </c>
+      <c r="E25">
+        <v>2011</v>
+      </c>
+      <c r="F25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" t="s">
+        <v>364</v>
+      </c>
+      <c r="H25" t="s">
+        <v>409</v>
+      </c>
+      <c r="I25">
+        <v>845</v>
+      </c>
+      <c r="J25" t="s">
+        <v>370</v>
+      </c>
+      <c r="K25">
+        <v>3</v>
+      </c>
+      <c r="L25">
+        <v>5302</v>
+      </c>
+      <c r="M25" s="41">
+        <f t="shared" si="0"/>
+        <v>9.034326669181441</v>
+      </c>
+      <c r="N25">
+        <v>42640</v>
+      </c>
+      <c r="O25" s="41">
+        <f t="shared" si="1"/>
+        <v>1.9887429643527206</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26">
+        <v>392</v>
+      </c>
+      <c r="B26">
+        <v>639</v>
+      </c>
+      <c r="C26">
+        <v>12529643</v>
+      </c>
+      <c r="D26" t="s">
+        <v>256</v>
+      </c>
+      <c r="E26">
+        <v>2003</v>
+      </c>
+      <c r="F26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" t="s">
+        <v>364</v>
+      </c>
+      <c r="H26" t="s">
+        <v>409</v>
+      </c>
+      <c r="I26">
+        <v>639</v>
+      </c>
+      <c r="L26">
+        <v>5302</v>
+      </c>
+      <c r="M26" s="41">
+        <f t="shared" si="0"/>
+        <v>7.3934364390795926</v>
+      </c>
+      <c r="N26">
+        <v>42640</v>
+      </c>
+      <c r="O26" s="41">
+        <f t="shared" si="1"/>
+        <v>1.4985928705440901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27">
+        <v>383</v>
+      </c>
+      <c r="B27">
+        <v>917</v>
+      </c>
+      <c r="C27">
+        <v>12445391</v>
+      </c>
+      <c r="D27" t="s">
+        <v>261</v>
+      </c>
+      <c r="E27">
+        <v>2002</v>
+      </c>
+      <c r="F27" t="s">
+        <v>188</v>
+      </c>
+      <c r="G27" t="s">
+        <v>364</v>
+      </c>
+      <c r="H27" t="s">
+        <v>409</v>
+      </c>
+      <c r="I27">
+        <v>917</v>
+      </c>
+      <c r="L27">
+        <v>5302</v>
+      </c>
+      <c r="M27" s="41">
+        <f t="shared" si="0"/>
+        <v>7.2236891738966431</v>
+      </c>
+      <c r="N27">
+        <v>42640</v>
+      </c>
+      <c r="O27" s="41">
+        <f t="shared" si="1"/>
+        <v>2.1505628517823641</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28">
+        <v>285</v>
+      </c>
+      <c r="B28">
+        <v>761</v>
+      </c>
+      <c r="C28">
+        <v>11099033</v>
+      </c>
+      <c r="D28" t="s">
+        <v>298</v>
+      </c>
+      <c r="E28">
+        <v>2000</v>
+      </c>
+      <c r="F28" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" t="s">
+        <v>364</v>
+      </c>
+      <c r="H28" t="s">
+        <v>409</v>
+      </c>
+      <c r="I28">
+        <v>761</v>
+      </c>
+      <c r="L28">
+        <v>5302</v>
+      </c>
+      <c r="M28" s="41">
+        <f t="shared" si="0"/>
+        <v>5.3753300641267447</v>
+      </c>
+      <c r="N28">
+        <v>42640</v>
+      </c>
+      <c r="O28" s="41">
+        <f t="shared" si="1"/>
+        <v>1.7847091932457788</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29">
+        <v>283</v>
+      </c>
+      <c r="B29">
+        <v>499</v>
+      </c>
+      <c r="C29">
+        <v>11099034</v>
+      </c>
+      <c r="D29" t="s">
+        <v>307</v>
+      </c>
+      <c r="E29">
+        <v>2000</v>
+      </c>
+      <c r="F29" t="s">
+        <v>128</v>
+      </c>
+      <c r="G29" t="s">
+        <v>364</v>
+      </c>
+      <c r="H29" t="s">
+        <v>409</v>
+      </c>
+      <c r="I29">
+        <v>498</v>
+      </c>
+      <c r="J29" t="s">
+        <v>370</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>5302</v>
+      </c>
+      <c r="M29" s="41">
+        <f t="shared" si="0"/>
+        <v>5.3376084496416443</v>
+      </c>
+      <c r="N29">
+        <v>42640</v>
+      </c>
+      <c r="O29" s="41">
+        <f t="shared" si="1"/>
+        <v>1.1702626641651031</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30">
+        <v>338</v>
+      </c>
+      <c r="B30">
+        <v>338</v>
+      </c>
+      <c r="C30">
+        <v>20422638</v>
+      </c>
+      <c r="D30" t="s">
+        <v>276</v>
+      </c>
+      <c r="E30">
+        <v>2010</v>
+      </c>
+      <c r="F30" t="s">
+        <v>277</v>
+      </c>
+      <c r="G30" t="s">
+        <v>368</v>
+      </c>
+      <c r="H30" t="s">
+        <v>417</v>
+      </c>
+      <c r="I30">
+        <v>338</v>
+      </c>
+      <c r="L30">
+        <v>1256</v>
+      </c>
+      <c r="M30" s="41">
+        <f t="shared" si="0"/>
+        <v>26.910828025477706</v>
+      </c>
+      <c r="N30">
+        <v>4545</v>
+      </c>
+      <c r="O30" s="41">
+        <f t="shared" si="1"/>
+        <v>7.4367436743674364</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31">
+        <v>413</v>
+      </c>
+      <c r="B31">
+        <v>456</v>
+      </c>
+      <c r="C31">
+        <v>18433294</v>
+      </c>
+      <c r="D31" t="s">
+        <v>244</v>
+      </c>
+      <c r="E31">
+        <v>2008</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" t="s">
+        <v>363</v>
+      </c>
+      <c r="H31" t="s">
+        <v>408</v>
+      </c>
+      <c r="I31">
+        <v>456</v>
+      </c>
+      <c r="L31">
+        <v>7501</v>
+      </c>
+      <c r="M31" s="41">
+        <f t="shared" si="0"/>
+        <v>5.5059325423276899</v>
+      </c>
+      <c r="N31">
+        <v>45836</v>
+      </c>
+      <c r="O31" s="41">
+        <f t="shared" si="1"/>
+        <v>0.99485120865695076</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32">
+        <v>319</v>
+      </c>
+      <c r="B32">
+        <v>329</v>
+      </c>
+      <c r="C32">
+        <v>16336044</v>
+      </c>
+      <c r="D32" t="s">
+        <v>281</v>
+      </c>
+      <c r="E32">
+        <v>2006</v>
+      </c>
+      <c r="F32" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" t="s">
+        <v>369</v>
+      </c>
+      <c r="H32" t="s">
+        <v>408</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>363</v>
+      </c>
+      <c r="K32">
+        <v>327</v>
+      </c>
+      <c r="L32">
+        <v>7501</v>
+      </c>
+      <c r="M32" s="41">
+        <f t="shared" si="0"/>
+        <v>4.2527662978269563</v>
+      </c>
+      <c r="N32">
+        <v>45836</v>
+      </c>
+      <c r="O32" s="41">
+        <f t="shared" si="1"/>
+        <v>0.71777642028100186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33">
+        <v>244</v>
+      </c>
+      <c r="B33">
+        <v>397</v>
+      </c>
+      <c r="C33">
+        <v>17412918</v>
+      </c>
+      <c r="D33" t="s">
+        <v>322</v>
+      </c>
+      <c r="E33">
+        <v>2007</v>
+      </c>
+      <c r="F33" t="s">
+        <v>323</v>
+      </c>
+      <c r="G33" t="s">
+        <v>363</v>
+      </c>
+      <c r="H33" t="s">
+        <v>408</v>
+      </c>
+      <c r="I33">
+        <v>397</v>
+      </c>
+      <c r="L33">
+        <v>7501</v>
+      </c>
+      <c r="M33" s="41">
+        <f t="shared" si="0"/>
+        <v>3.2528996133848818</v>
+      </c>
+      <c r="N33">
+        <v>45836</v>
+      </c>
+      <c r="O33" s="41">
+        <f t="shared" si="1"/>
+        <v>0.86613142508072261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34">
+        <v>242</v>
+      </c>
+      <c r="B34">
+        <v>397</v>
+      </c>
+      <c r="C34">
+        <v>18981222</v>
+      </c>
+      <c r="D34" t="s">
+        <v>348</v>
+      </c>
+      <c r="E34">
+        <v>2009</v>
+      </c>
+      <c r="F34" t="s">
+        <v>349</v>
+      </c>
+      <c r="G34" t="s">
+        <v>363</v>
+      </c>
+      <c r="H34" t="s">
+        <v>408</v>
+      </c>
+      <c r="I34">
+        <v>397</v>
+      </c>
+      <c r="L34">
+        <v>7501</v>
+      </c>
+      <c r="M34" s="41">
+        <f t="shared" ref="M34:M65" si="2">A34/L34*100</f>
+        <v>3.2262365017997596</v>
+      </c>
+      <c r="N34">
+        <v>45836</v>
+      </c>
+      <c r="O34" s="41">
+        <f t="shared" ref="O34:O65" si="3">B34/N34*100</f>
+        <v>0.86613142508072261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35">
+        <v>4937</v>
+      </c>
+      <c r="B35">
+        <v>11050</v>
+      </c>
+      <c r="C35">
+        <v>18029348</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35">
+        <v>2008</v>
+      </c>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" t="s">
+        <v>361</v>
+      </c>
+      <c r="H35" t="s">
+        <v>406</v>
+      </c>
+      <c r="I35">
+        <v>11050</v>
+      </c>
+      <c r="L35">
+        <v>11521</v>
+      </c>
+      <c r="M35" s="41">
+        <f t="shared" si="2"/>
+        <v>42.852182970228284</v>
+      </c>
+      <c r="N35">
+        <v>72762</v>
+      </c>
+      <c r="O35" s="41">
+        <f t="shared" si="3"/>
+        <v>15.186498446991562</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36">
+        <v>465</v>
+      </c>
+      <c r="B36">
+        <v>468</v>
+      </c>
+      <c r="C36">
+        <v>11256614</v>
+      </c>
+      <c r="D36" t="s">
+        <v>222</v>
+      </c>
+      <c r="E36">
+        <v>2000</v>
+      </c>
+      <c r="F36" t="s">
+        <v>223</v>
+      </c>
+      <c r="G36" t="s">
+        <v>361</v>
+      </c>
+      <c r="H36" t="s">
+        <v>406</v>
+      </c>
+      <c r="I36">
+        <v>468</v>
+      </c>
+      <c r="L36">
+        <v>11521</v>
+      </c>
+      <c r="M36" s="41">
+        <f t="shared" si="2"/>
+        <v>4.0361079767381307</v>
+      </c>
+      <c r="N36">
+        <v>72762</v>
+      </c>
+      <c r="O36" s="41">
+        <f t="shared" si="3"/>
+        <v>0.64319287540199555</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37">
+        <v>343</v>
+      </c>
+      <c r="B37">
+        <v>509</v>
+      </c>
+      <c r="C37">
+        <v>16189514</v>
+      </c>
+      <c r="D37" t="s">
+        <v>273</v>
+      </c>
+      <c r="E37">
+        <v>2005</v>
+      </c>
+      <c r="F37" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37" t="s">
+        <v>361</v>
+      </c>
+      <c r="H37" t="s">
+        <v>406</v>
+      </c>
+      <c r="I37">
+        <v>509</v>
+      </c>
+      <c r="L37">
+        <v>11521</v>
+      </c>
+      <c r="M37" s="41">
+        <f t="shared" si="2"/>
+        <v>2.9771721204756534</v>
+      </c>
+      <c r="N37">
+        <v>72762</v>
+      </c>
+      <c r="O37" s="41">
+        <f t="shared" si="3"/>
+        <v>0.69954096918721309</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38">
+        <v>2412</v>
+      </c>
+      <c r="B38">
+        <v>2412</v>
+      </c>
+      <c r="C38">
+        <v>18614015</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38">
+        <v>2008</v>
+      </c>
+      <c r="F38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" t="s">
+        <v>360</v>
+      </c>
+      <c r="H38" t="s">
+        <v>405</v>
+      </c>
+      <c r="I38">
+        <v>2412</v>
+      </c>
+      <c r="L38">
+        <v>22068</v>
+      </c>
+      <c r="M38" s="41">
+        <f t="shared" si="2"/>
+        <v>10.929853181076671</v>
+      </c>
+      <c r="N38">
+        <v>178024</v>
+      </c>
+      <c r="O38" s="41">
+        <f t="shared" si="3"/>
+        <v>1.3548735002022199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39">
+        <v>1186</v>
+      </c>
+      <c r="B39">
+        <v>1213</v>
+      </c>
+      <c r="C39">
+        <v>14651853</v>
+      </c>
+      <c r="D39" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39">
+        <v>2003</v>
+      </c>
+      <c r="F39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" t="s">
+        <v>360</v>
+      </c>
+      <c r="H39" t="s">
+        <v>405</v>
+      </c>
+      <c r="I39">
+        <v>1213</v>
+      </c>
+      <c r="L39">
+        <v>22068</v>
+      </c>
+      <c r="M39" s="41">
+        <f t="shared" si="2"/>
+        <v>5.3742976255211161</v>
+      </c>
+      <c r="N39">
+        <v>178024</v>
+      </c>
+      <c r="O39" s="41">
+        <f t="shared" si="3"/>
+        <v>0.68136880420617452</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40">
+        <v>375</v>
+      </c>
+      <c r="B40">
+        <v>375</v>
+      </c>
+      <c r="C40">
+        <v>12865426</v>
+      </c>
+      <c r="D40" t="s">
+        <v>269</v>
+      </c>
+      <c r="E40">
+        <v>2003</v>
+      </c>
+      <c r="F40" t="s">
+        <v>270</v>
+      </c>
+      <c r="G40" t="s">
+        <v>360</v>
+      </c>
+      <c r="H40" t="s">
+        <v>405</v>
+      </c>
+      <c r="I40">
+        <v>375</v>
+      </c>
+      <c r="L40">
+        <v>22068</v>
+      </c>
+      <c r="M40" s="41">
+        <f t="shared" si="2"/>
+        <v>1.6992930940728659</v>
+      </c>
+      <c r="N40">
+        <v>178024</v>
+      </c>
+      <c r="O40" s="41">
+        <f t="shared" si="3"/>
+        <v>0.21064575562845458</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41">
+        <v>266</v>
+      </c>
+      <c r="B41">
+        <v>433</v>
+      </c>
+      <c r="C41">
+        <v>11591653</v>
+      </c>
+      <c r="D41" t="s">
+        <v>308</v>
+      </c>
+      <c r="E41">
+        <v>2001</v>
+      </c>
+      <c r="F41" t="s">
+        <v>170</v>
+      </c>
+      <c r="G41" t="s">
+        <v>360</v>
+      </c>
+      <c r="H41" t="s">
+        <v>405</v>
+      </c>
+      <c r="I41">
+        <v>433</v>
+      </c>
+      <c r="L41">
+        <v>22068</v>
+      </c>
+      <c r="M41" s="41">
+        <f t="shared" si="2"/>
+        <v>1.2053652347290194</v>
+      </c>
+      <c r="N41">
+        <v>178024</v>
+      </c>
+      <c r="O41" s="41">
+        <f t="shared" si="3"/>
+        <v>0.2432256324989889</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42">
+        <v>1043</v>
+      </c>
+      <c r="B42">
+        <v>1365</v>
+      </c>
+      <c r="C42">
+        <v>15525680</v>
+      </c>
+      <c r="D42" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42">
+        <v>2005</v>
+      </c>
+      <c r="F42" t="s">
+        <v>164</v>
+      </c>
+      <c r="G42" t="s">
+        <v>367</v>
+      </c>
+      <c r="H42" t="s">
+        <v>415</v>
+      </c>
+      <c r="I42">
+        <v>1365</v>
+      </c>
+      <c r="L42">
+        <v>2317</v>
+      </c>
+      <c r="M42" s="41">
+        <f t="shared" si="2"/>
+        <v>45.015105740181269</v>
+      </c>
+      <c r="N42">
+        <v>6928</v>
+      </c>
+      <c r="O42" s="41">
+        <f t="shared" si="3"/>
+        <v>19.702655889145497</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43">
+        <v>735</v>
+      </c>
+      <c r="B43">
+        <v>735</v>
+      </c>
+      <c r="C43">
+        <v>14532352</v>
+      </c>
+      <c r="D43" t="s">
+        <v>179</v>
+      </c>
+      <c r="E43">
+        <v>2003</v>
+      </c>
+      <c r="F43" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" t="s">
+        <v>367</v>
+      </c>
+      <c r="H43" t="s">
+        <v>415</v>
+      </c>
+      <c r="I43">
+        <v>735</v>
+      </c>
+      <c r="L43">
+        <v>2317</v>
+      </c>
+      <c r="M43" s="41">
+        <f t="shared" si="2"/>
+        <v>31.722054380664655</v>
+      </c>
+      <c r="N43">
+        <v>6928</v>
+      </c>
+      <c r="O43" s="41">
+        <f t="shared" si="3"/>
+        <v>10.609122401847575</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44">
+        <v>613</v>
+      </c>
+      <c r="B44">
+        <v>613</v>
+      </c>
+      <c r="C44">
+        <v>12657046</v>
+      </c>
+      <c r="D44" t="s">
+        <v>189</v>
+      </c>
+      <c r="E44">
+        <v>2003</v>
+      </c>
+      <c r="F44" t="s">
+        <v>190</v>
+      </c>
+      <c r="G44" t="s">
+        <v>367</v>
+      </c>
+      <c r="H44" t="s">
+        <v>415</v>
+      </c>
+      <c r="I44">
+        <v>613</v>
+      </c>
+      <c r="L44">
+        <v>2317</v>
+      </c>
+      <c r="M44" s="41">
+        <f t="shared" si="2"/>
+        <v>26.456624946050926</v>
+      </c>
+      <c r="N44">
+        <v>6928</v>
+      </c>
+      <c r="O44" s="41">
+        <f t="shared" si="3"/>
+        <v>8.8481524249422634</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45">
+        <v>4247</v>
+      </c>
+      <c r="B45">
+        <v>7046</v>
+      </c>
+      <c r="C45">
+        <v>16823372</v>
+      </c>
+      <c r="D45" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45">
+        <v>2006</v>
+      </c>
+      <c r="F45" t="s">
+        <v>55</v>
+      </c>
+      <c r="G45" t="s">
+        <v>366</v>
+      </c>
+      <c r="H45" t="s">
+        <v>429</v>
+      </c>
+      <c r="I45">
+        <v>7043</v>
+      </c>
+      <c r="J45" t="s">
+        <v>371</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="L45">
+        <v>4507</v>
+      </c>
+      <c r="M45" s="41">
+        <f t="shared" si="2"/>
+        <v>94.231195917461733</v>
+      </c>
+      <c r="N45">
+        <v>15733</v>
+      </c>
+      <c r="O45" s="41">
+        <f t="shared" si="3"/>
+        <v>44.784847136591878</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46">
+        <v>258</v>
+      </c>
+      <c r="B46">
+        <v>259</v>
+      </c>
+      <c r="C46">
+        <v>12529438</v>
+      </c>
+      <c r="D46" t="s">
+        <v>313</v>
+      </c>
+      <c r="E46">
+        <v>2003</v>
+      </c>
+      <c r="F46" t="s">
+        <v>164</v>
+      </c>
+      <c r="G46" t="s">
+        <v>366</v>
+      </c>
+      <c r="H46" t="s">
+        <v>429</v>
+      </c>
+      <c r="I46">
+        <v>259</v>
+      </c>
+      <c r="L46">
+        <v>4507</v>
+      </c>
+      <c r="M46" s="41">
+        <f t="shared" si="2"/>
+        <v>5.7244286665187483</v>
+      </c>
+      <c r="N46">
+        <v>15733</v>
+      </c>
+      <c r="O46" s="41">
+        <f t="shared" si="3"/>
+        <v>1.6462213182482679</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47">
+        <v>1406</v>
+      </c>
+      <c r="B47">
+        <v>1863</v>
+      </c>
+      <c r="C47">
+        <v>14562095</v>
+      </c>
+      <c r="D47" t="s">
+        <v>127</v>
+      </c>
+      <c r="E47">
+        <v>2003</v>
+      </c>
+      <c r="F47" t="s">
+        <v>128</v>
+      </c>
+      <c r="G47" t="s">
+        <v>365</v>
+      </c>
+      <c r="H47" t="s">
+        <v>410</v>
+      </c>
+      <c r="I47">
+        <v>1863</v>
+      </c>
+      <c r="L47">
+        <v>5086</v>
+      </c>
+      <c r="M47" s="41">
+        <f t="shared" si="2"/>
+        <v>27.644514353126233</v>
+      </c>
+      <c r="N47">
+        <v>34276</v>
+      </c>
+      <c r="O47" s="41">
+        <f t="shared" si="3"/>
+        <v>5.4352899988330021</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="A48">
+        <v>845</v>
+      </c>
+      <c r="B48">
+        <v>845</v>
+      </c>
+      <c r="C48">
+        <v>16823961</v>
+      </c>
+      <c r="D48" t="s">
+        <v>175</v>
+      </c>
+      <c r="E48">
+        <v>2006</v>
+      </c>
+      <c r="F48" t="s">
+        <v>168</v>
+      </c>
+      <c r="G48" t="s">
+        <v>365</v>
+      </c>
+      <c r="H48" t="s">
+        <v>410</v>
+      </c>
+      <c r="I48">
+        <v>845</v>
+      </c>
+      <c r="L48">
+        <v>5086</v>
+      </c>
+      <c r="M48" s="41">
+        <f t="shared" si="2"/>
+        <v>16.614235155328352</v>
+      </c>
+      <c r="N48">
+        <v>34276</v>
+      </c>
+      <c r="O48" s="41">
+        <f t="shared" si="3"/>
+        <v>2.4652818298517913</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49">
+        <v>503</v>
+      </c>
+      <c r="B49">
+        <v>503</v>
+      </c>
+      <c r="C49">
+        <v>14576278</v>
+      </c>
+      <c r="D49" t="s">
+        <v>207</v>
+      </c>
+      <c r="E49">
+        <v>2003</v>
+      </c>
+      <c r="F49" t="s">
+        <v>208</v>
+      </c>
+      <c r="G49" t="s">
+        <v>365</v>
+      </c>
+      <c r="H49" t="s">
+        <v>410</v>
+      </c>
+      <c r="I49">
+        <v>503</v>
+      </c>
+      <c r="L49">
+        <v>5086</v>
+      </c>
+      <c r="M49" s="41">
+        <f t="shared" si="2"/>
+        <v>9.8898938261895406</v>
+      </c>
+      <c r="N49">
+        <v>34276</v>
+      </c>
+      <c r="O49" s="41">
+        <f t="shared" si="3"/>
+        <v>1.4674991247520131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50">
+        <v>498</v>
+      </c>
+      <c r="B50">
+        <v>638</v>
+      </c>
+      <c r="C50">
+        <v>16429126</v>
+      </c>
+      <c r="D50" t="s">
+        <v>209</v>
+      </c>
+      <c r="E50">
+        <v>2006</v>
+      </c>
+      <c r="F50" t="s">
+        <v>128</v>
+      </c>
+      <c r="G50" t="s">
+        <v>365</v>
+      </c>
+      <c r="H50" t="s">
+        <v>410</v>
+      </c>
+      <c r="I50">
+        <v>638</v>
+      </c>
+      <c r="L50">
+        <v>5086</v>
+      </c>
+      <c r="M50" s="41">
+        <f t="shared" si="2"/>
+        <v>9.7915847424302012</v>
+      </c>
+      <c r="N50">
+        <v>34276</v>
+      </c>
+      <c r="O50" s="41">
+        <f t="shared" si="3"/>
+        <v>1.8613607188703467</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51">
+        <v>290</v>
+      </c>
+      <c r="B51">
+        <v>331</v>
+      </c>
+      <c r="C51">
+        <v>11914276</v>
+      </c>
+      <c r="D51" t="s">
+        <v>296</v>
+      </c>
+      <c r="E51">
+        <v>2002</v>
+      </c>
+      <c r="F51" t="s">
+        <v>297</v>
+      </c>
+      <c r="G51" t="s">
+        <v>365</v>
+      </c>
+      <c r="H51" t="s">
+        <v>410</v>
+      </c>
+      <c r="I51">
+        <v>331</v>
+      </c>
+      <c r="L51">
+        <v>5086</v>
+      </c>
+      <c r="M51" s="41">
+        <f t="shared" si="2"/>
+        <v>5.7019268580416833</v>
+      </c>
+      <c r="N51">
+        <v>34276</v>
+      </c>
+      <c r="O51" s="41">
+        <f t="shared" si="3"/>
+        <v>0.96569027891235848</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:O51">
+    <sortCondition ref="H2:H51"/>
+  </sortState>
+  <conditionalFormatting sqref="M1:M51">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThanOrEqual">
+      <formula>20</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+      <formula>30</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThanOrEqual">
+      <formula>60</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O51">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+      <formula>20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>